<commit_message>
Watering Apparatus tested, build TempHumditControl
</commit_message>
<xml_diff>
--- a/SensorModel/piecewise interpolation.xlsx
+++ b/SensorModel/piecewise interpolation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1040" windowWidth="24480" windowHeight="15720" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="0" windowWidth="24480" windowHeight="17260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -335,7 +335,12 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.523078302712161"/>
+                  <c:y val="-0.326662917135358"/>
+                </c:manualLayout>
+              </c:layout>
               <c:numFmt formatCode="0.000000E+00" sourceLinked="0"/>
             </c:trendlineLbl>
           </c:trendline>
@@ -845,7 +850,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>